<commit_message>
fruit veg update 2
J'ai refais les images de plusieurs (probleme de transparence)
</commit_message>
<xml_diff>
--- a/Squelette_sujet1.xlsx
+++ b/Squelette_sujet1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="88">
   <si>
     <t>Var1_1</t>
   </si>
@@ -297,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -317,11 +317,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -335,6 +337,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,144 +351,144 @@
   <dimension ref="A1:H49"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="true"/>
-    <col min="2" max="2" width="7.140625" customWidth="true"/>
-    <col min="3" max="3" width="7.140625" customWidth="true"/>
+    <col min="1" max="1" width="18.28515625" customWidth="true"/>
+    <col min="2" max="2" width="9.28515625" customWidth="true"/>
+    <col min="3" max="3" width="9.140625" customWidth="true"/>
     <col min="4" max="4" width="7.140625" customWidth="true"/>
-    <col min="5" max="5" width="7.140625" customWidth="true"/>
-    <col min="6" max="6" width="7.140625" customWidth="true"/>
+    <col min="5" max="5" width="10" customWidth="true"/>
+    <col min="6" max="6" width="9.7109375" customWidth="true"/>
     <col min="7" max="7" width="7.140625" customWidth="true"/>
     <col min="8" max="8" width="7.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>54</v>
+      <c r="C2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="F2">
-        <v>0.68906150013208389</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>44</v>
+        <v>1.9777747000007366</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>27</v>
+      <c r="B3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="F3">
-        <v>0.20506130019202828</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>45</v>
+        <v>0.30028690000017377</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>0.69291440000051807</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4">
-        <v>0.27956689987331629</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
+      <c r="E5" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="F5">
-        <v>0.36183449998497963</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>45</v>
+        <v>1.1078081000005113</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
YOOOO on a le titre des axes sur le tableau excel
</commit_message>
<xml_diff>
--- a/Squelette_sujet1.xlsx
+++ b/Squelette_sujet1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="96">
   <si>
     <t>Var1_1</t>
   </si>
@@ -277,6 +277,30 @@
   </si>
   <si>
     <t>Squelette_sujet1_48</t>
+  </si>
+  <si>
+    <t>Stimulus</t>
+  </si>
+  <si>
+    <t>Déterminant_Mot</t>
+  </si>
+  <si>
+    <t>Nom_Mot</t>
+  </si>
+  <si>
+    <t>Déterminant_image</t>
+  </si>
+  <si>
+    <t>Nom_Image</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Lettre</t>
+  </si>
+  <si>
+    <t>Congruence</t>
   </si>
 </sst>
 </file>
@@ -297,7 +321,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -319,11 +343,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -339,6 +369,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,377 +388,377 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="true"/>
-    <col min="2" max="2" width="9.28515625" customWidth="true"/>
-    <col min="3" max="3" width="9.140625" customWidth="true"/>
-    <col min="4" max="4" width="7.140625" customWidth="true"/>
-    <col min="5" max="5" width="10" customWidth="true"/>
+    <col min="2" max="2" width="17" customWidth="true"/>
+    <col min="3" max="3" width="10" customWidth="true"/>
+    <col min="4" max="4" width="18.85546875" customWidth="true"/>
+    <col min="5" max="5" width="11.85546875" customWidth="true"/>
     <col min="6" max="6" width="9.7109375" customWidth="true"/>
-    <col min="7" max="7" width="7.140625" customWidth="true"/>
-    <col min="8" max="8" width="7.140625" customWidth="true"/>
+    <col min="7" max="7" width="6.42578125" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>46</v>
+      <c r="A1" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>1.2207727003842592</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>0.35280170012265444</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4">
+        <v>0.21127720037475228</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="F5">
+        <v>0.26154580013826489</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F2">
-        <v>1.9777747000007366</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="D6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <v>0.45584670035168529</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <v>0.24809789983555675</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>1.0437461999244988</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9">
+        <v>0.28163790004327893</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10">
+        <v>0.19671649998053908</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>0.25361139979213476</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>0.30028690000017377</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4">
-        <v>0.69291440000051807</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5">
-        <v>1.1078081000005113</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>0.19721479993313551</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="C12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7">
-        <v>0.24037609994411469</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="E12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="F12">
+        <v>0.73745060013607144</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13">
+        <v>0.22410959983244538</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8">
-        <v>0.3230805997736752</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9">
-        <v>0.19921790016815066</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10">
-        <v>0.13335869973525405</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11">
-        <v>0.1956432000733912</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12">
-        <v>0.2842123000882566</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13">
-        <v>0.32076150039210916</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>28</v>
+      <c r="E14" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="F14">
-        <v>0.78020629985257983</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>45</v>
+        <v>0.23413520026952028</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="H14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">

</xml_diff>